<commit_message>
working on chart data
</commit_message>
<xml_diff>
--- a/Python/src/_Highlands/questions.xlsx
+++ b/Python/src/_Highlands/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Question</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Once a quarter</t>
   </si>
   <si>
-    <t>Q1 Thinking as the CEO of your client, what will they say about their relationship with your company?</t>
-  </si>
-  <si>
     <t>Their CEO loves you and your company</t>
   </si>
   <si>
@@ -78,27 +75,15 @@
     <t>Their CEO does not know you (personally, or anyone in your company)</t>
   </si>
   <si>
-    <t>Q2 As you think of the business relationship with your client, which of the following best describes the time you spend with them discussing their business?</t>
-  </si>
-  <si>
     <t>radio</t>
   </si>
   <si>
     <t>text</t>
   </si>
   <si>
-    <t>graph</t>
-  </si>
-  <si>
-    <t>table</t>
-  </si>
-  <si>
     <t>Once a half year or less</t>
   </si>
   <si>
-    <t>Q3a What is your understanding of how your client would react to you working with their other suppliers (that you may commonly refer to as a "competitor") to help them (the client) with their business?</t>
-  </si>
-  <si>
     <t>Do not believe it is possible</t>
   </si>
   <si>
@@ -111,129 +96,15 @@
     <t>They would want to engage with such a team</t>
   </si>
   <si>
-    <t>Q3b Considering your response to Q3a, do you know why they would say that?</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Q3c Again, with reference to Q3a, does your client see the value and want to do this?</t>
-  </si>
-  <si>
     <t>I do know at this time</t>
   </si>
   <si>
-    <t>Q3d Thinking like the client, and reflecting on your responses to Q3a to Q3c, do you understand the benefits to your client?</t>
-  </si>
-  <si>
-    <t>Q3e Looking at your answers from Q3a to Q3d inclusive, would your 1st or 2nd line manager agree with you?</t>
-  </si>
-  <si>
-    <t>Do not know</t>
-  </si>
-  <si>
-    <t>Q3f Has your 1st line or 2nd line manager agreed with you in real time as you answered?</t>
-  </si>
-  <si>
-    <t>Q4a Is there a board member in your company that is or would be, an executive sponsor for this type of relationship?</t>
-  </si>
-  <si>
-    <t>Q4b If Q4a was answered "No", does the sponsor or potential sponsor report to your board?</t>
-  </si>
-  <si>
-    <t>Q4c How many times a year does your executive sponsor meet with your "competitor"?</t>
-  </si>
-  <si>
-    <t>Does not meet</t>
-  </si>
-  <si>
-    <t>1 to 3</t>
-  </si>
-  <si>
-    <t>3 to 5</t>
-  </si>
-  <si>
-    <t>More than 5 times a year</t>
-  </si>
-  <si>
-    <t>I do not know</t>
-  </si>
-  <si>
-    <t>Q4d How often does your sponsor talk informally with their counterpart in your "competitor"?</t>
-  </si>
-  <si>
-    <t>Weekly</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>Quarterly</t>
-  </si>
-  <si>
-    <t>Annually</t>
-  </si>
-  <si>
-    <t>Q6a What does your client sell today, that drives most of their sales?</t>
-  </si>
-  <si>
-    <t>The client sells services / consulting</t>
-  </si>
-  <si>
-    <t>The client sells products</t>
-  </si>
-  <si>
-    <t>The client sells both services and products</t>
-  </si>
-  <si>
-    <t>The client is a non profit organization</t>
-  </si>
-  <si>
-    <t>Q8a  Thinking about your company's overall credibility &amp; trust,  have there been any issues that have affected this in the past 12 month or more recently?</t>
-  </si>
-  <si>
-    <t>rows</t>
-  </si>
-  <si>
-    <t>columns</t>
-  </si>
-  <si>
-    <t>Last 30 days</t>
-  </si>
-  <si>
-    <t>Last 90 days</t>
-  </si>
-  <si>
-    <t>Last 180 days</t>
-  </si>
-  <si>
-    <t>In the past year</t>
-  </si>
-  <si>
-    <t>Extremely serious</t>
-  </si>
-  <si>
-    <t>Significant but quickly resolved</t>
-  </si>
-  <si>
-    <t>Minor</t>
-  </si>
-  <si>
-    <t>Q12a Thinking like your client, what new business outcomes do they need to obtain to grow their business?</t>
-  </si>
-  <si>
-    <t>Please describe the business impact in terms of how it will impact key business measurements of importance to their board.</t>
-  </si>
-  <si>
-    <t>Q10  Where is your client's business dynamic vs the market dynamic?</t>
-  </si>
-  <si>
-    <t>Please enter "X,Y"  (X = Market Growth), Y = Client Revenue Growth): Major Decline = 0, Flat = 5, Very Strong = 10</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -264,34 +135,28 @@
     <t>This is the Highlands Client Teaming Assessment.  It will help establish the likelihood of a Sales Trinity being created and then delivering a True Business Solution.   Version Draft2.3</t>
   </si>
   <si>
-    <t>What Client are you assessing?</t>
-  </si>
-  <si>
-    <t>At the end of this questionnaire you will be asked if you want to complete a new form, allowing you to profile another client.</t>
-  </si>
-  <si>
-    <t>Name of client to profile</t>
-  </si>
-  <si>
-    <t>Client location</t>
-  </si>
-  <si>
-    <t>Exploring Relationships</t>
-  </si>
-  <si>
-    <t>This series of questions explores the relationships between you, your "competitor" and the client. These questions help to quantify who knows who and the level of trust and confidence that exists in those relationships.</t>
-  </si>
-  <si>
-    <t>Business Situation</t>
-  </si>
-  <si>
-    <t>This section contains a series of questions to understand the business dynamics of your client</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>autofill</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Again, with reference to 8, does your client see the value and want to do this?</t>
+  </si>
+  <si>
+    <t>What is your understanding of how your client would react to you working with their other suppliers (that you may commonly refer to as a "competitor") to help them (the client) with their business?</t>
+  </si>
+  <si>
+    <t>As you think of the business relationship with your client, which of the following best describes the time you spend with them discussing their business?</t>
+  </si>
+  <si>
+    <t>Thinking as the CEO of your client, what will they say about their relationship with your company?</t>
+  </si>
+  <si>
+    <t>Considering your response to 8, do you know why they would say that?</t>
   </si>
 </sst>
 </file>
@@ -421,8 +286,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -574,7 +443,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -630,6 +499,8 @@
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -685,6 +556,8 @@
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1014,626 +887,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P111"/>
+  <dimension ref="A1:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="13" width="28.33203125" customWidth="1"/>
+    <col min="2" max="14" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23">
+    <row r="1" spans="1:12" ht="23">
       <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:12" ht="16">
       <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="16"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
-      <c r="J3" s="1"/>
+      <c r="D3" s="16"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" ht="17">
-      <c r="A4" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="J4" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="17">
+      <c r="B4" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="16"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="17">
-      <c r="A5" s="18"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="17">
+      <c r="B5" s="18"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="17">
-      <c r="A6" s="18"/>
-      <c r="B6" s="16"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="17">
+      <c r="B6" s="18"/>
       <c r="C6" s="16"/>
-      <c r="J6" s="1"/>
+      <c r="D6" s="16"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="17">
-      <c r="A7" s="18"/>
-      <c r="B7" s="16"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="17">
+      <c r="B7" s="18"/>
       <c r="C7" s="16"/>
-      <c r="J7" s="1"/>
+      <c r="D7" s="16"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" ht="17">
-      <c r="A8" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>89</v>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="17">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" ht="17">
-      <c r="A9" s="18"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="17">
+      <c r="B9" s="18"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="17">
-      <c r="A10" s="18"/>
-      <c r="B10" s="16"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="17">
+      <c r="B10" s="18"/>
       <c r="C10" s="16"/>
-      <c r="J10" s="1"/>
+      <c r="D10" s="16"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" ht="17">
-      <c r="A11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>21</v>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="17">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" ht="17">
-      <c r="A12" s="18"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="17">
+      <c r="B12" s="18"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" ht="17">
-      <c r="A13" s="18"/>
-      <c r="B13" s="16"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="17">
+      <c r="B13" s="18"/>
       <c r="C13" s="16"/>
-      <c r="J13" s="1"/>
+      <c r="D13" s="16"/>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" ht="17">
-      <c r="A14" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="J14" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="17">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" ht="17">
-      <c r="A15" s="18"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J15" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="17">
+      <c r="B15" s="18"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" ht="17">
-      <c r="A16" s="18"/>
-      <c r="B16" s="16"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="17">
+      <c r="B16" s="18"/>
       <c r="C16" s="16"/>
-      <c r="J16" s="1"/>
+      <c r="D16" s="16"/>
       <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" ht="17">
-      <c r="A17" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="J17" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" ht="17">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" ht="17">
-      <c r="A18" s="18"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J18" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" ht="17">
+      <c r="B18" s="18"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" ht="17">
-      <c r="A19" s="18"/>
-      <c r="B19" s="16"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" ht="17">
+      <c r="B19" s="18"/>
       <c r="C19" s="16"/>
-      <c r="J19" s="1"/>
+      <c r="D19" s="16"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" ht="17">
-      <c r="A20" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="J20" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" ht="17">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="16"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12">
       <c r="B21" s="16"/>
-      <c r="C21" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J21" s="1"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="16"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
-      <c r="J22" s="1"/>
+      <c r="D22" s="16"/>
       <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" ht="17">
-      <c r="A23" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>78</v>
-      </c>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" ht="17">
+      <c r="B23" s="18"/>
       <c r="C23" s="16"/>
-      <c r="J23" s="1"/>
+      <c r="D23" s="16"/>
       <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="16"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="B24" s="16"/>
-      <c r="C24" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="J24" s="1"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
       <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="16"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
-      <c r="J25" s="1"/>
+      <c r="D25" s="16"/>
       <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" ht="17">
-      <c r="A26" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>21</v>
-      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" ht="17">
+      <c r="B26" s="18"/>
       <c r="C26" s="16"/>
-      <c r="J26" s="1"/>
+      <c r="D26" s="16"/>
       <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" ht="17">
-      <c r="A27" s="18"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J27" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" ht="17">
+      <c r="B27" s="18"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
       <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" ht="17">
-      <c r="A28" s="18"/>
-      <c r="B28" s="16"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" ht="17">
+      <c r="B28" s="18"/>
       <c r="C28" s="16"/>
-      <c r="J28" s="1"/>
+      <c r="D28" s="16"/>
       <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" ht="17">
-      <c r="A29" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>21</v>
-      </c>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" ht="17">
+      <c r="B29" s="18"/>
       <c r="C29" s="16"/>
-      <c r="J29" s="1"/>
+      <c r="D29" s="16"/>
       <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="16"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="B30" s="16"/>
-      <c r="C30" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J30" s="1"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
       <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="C31" s="16"/>
-      <c r="J31" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="D31" s="16"/>
       <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" ht="17">
-      <c r="A32" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>78</v>
-      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" ht="17">
+      <c r="B32" s="18"/>
       <c r="C32" s="16"/>
-      <c r="J32" s="1"/>
+      <c r="D32" s="16"/>
       <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="1:16" ht="16">
-      <c r="A33" s="17"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:17" ht="16">
       <c r="B33" s="17"/>
-      <c r="C33" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="14"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="13"/>
+      <c r="F33" s="14"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="1"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="5"/>
       <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="1:16" ht="16">
-      <c r="A34" s="17"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:17" ht="16">
       <c r="B34" s="17"/>
-      <c r="C34" s="14"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
-      <c r="F34" s="13"/>
+      <c r="F34" s="14"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="1"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="5"/>
       <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="1:16" ht="17">
-      <c r="A35" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="12"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:17" ht="17">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="7"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="8"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="6"/>
+      <c r="L35" s="7"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
-    </row>
-    <row r="36" spans="1:16" ht="17">
-      <c r="A36" s="9"/>
+      <c r="Q35" s="6"/>
+    </row>
+    <row r="36" spans="1:17" ht="17">
       <c r="B36" s="9"/>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="9"/>
+      <c r="D36" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="F36" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="7"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="8"/>
       <c r="K36" s="7"/>
-      <c r="L36" s="6"/>
+      <c r="L36" s="7"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
-    </row>
-    <row r="37" spans="1:16" ht="17">
-      <c r="A37" s="9"/>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="37" spans="1:17" ht="17">
       <c r="B37" s="9"/>
-      <c r="C37" s="12">
+      <c r="C37" s="9"/>
+      <c r="D37" s="12">
         <v>9</v>
       </c>
-      <c r="D37" s="12">
+      <c r="E37" s="12">
         <v>3</v>
       </c>
-      <c r="E37" s="12">
+      <c r="F37" s="12">
         <v>0</v>
       </c>
-      <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="7"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="8"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="6"/>
+      <c r="L37" s="7"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
-    </row>
-    <row r="38" spans="1:16" ht="17">
-      <c r="A38" s="9"/>
+      <c r="Q37" s="6"/>
+    </row>
+    <row r="38" spans="1:17" ht="17">
       <c r="B38" s="9"/>
-      <c r="C38" s="12"/>
+      <c r="C38" s="9"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="7"/>
+      <c r="I38" s="12"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
-      <c r="L38" s="6"/>
+      <c r="L38" s="7"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
-    </row>
-    <row r="39" spans="1:16" ht="17">
-      <c r="A39" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="12"/>
+      <c r="Q38" s="6"/>
+    </row>
+    <row r="39" spans="1:17" ht="17">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="7"/>
+      <c r="I39" s="12"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
-      <c r="L39" s="6"/>
+      <c r="L39" s="7"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
-    </row>
-    <row r="40" spans="1:16" ht="17">
-      <c r="A40" s="10"/>
+      <c r="Q39" s="6"/>
+    </row>
+    <row r="40" spans="1:17" ht="17">
       <c r="B40" s="10"/>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10"/>
+      <c r="D40" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="G40" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="H40" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I40" s="7"/>
+      <c r="I40" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
-      <c r="L40" s="6"/>
+      <c r="L40" s="7"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
-    </row>
-    <row r="41" spans="1:16" ht="17">
-      <c r="A41" s="9"/>
+      <c r="Q40" s="6"/>
+    </row>
+    <row r="41" spans="1:17" ht="17">
       <c r="B41" s="9"/>
-      <c r="C41" s="12">
+      <c r="C41" s="9"/>
+      <c r="D41" s="12">
         <v>7</v>
       </c>
-      <c r="D41" s="8">
+      <c r="E41" s="8">
         <v>4</v>
       </c>
-      <c r="E41" s="8">
+      <c r="F41" s="8">
         <v>3</v>
       </c>
-      <c r="F41" s="8">
+      <c r="G41" s="8">
         <v>2</v>
       </c>
-      <c r="G41" s="8">
+      <c r="H41" s="8">
         <v>1</v>
       </c>
-      <c r="H41" s="8">
+      <c r="I41" s="8">
         <v>0</v>
       </c>
-      <c r="I41" s="8"/>
       <c r="J41" s="8"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="6"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="7"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
-    </row>
-    <row r="42" spans="1:16" ht="17">
-      <c r="A42" s="9"/>
+      <c r="Q41" s="6"/>
+    </row>
+    <row r="42" spans="1:17" ht="17">
       <c r="B42" s="9"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="8"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="12"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="6"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="7"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
-    </row>
-    <row r="43" spans="1:16" ht="17">
-      <c r="A43" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="8"/>
+      <c r="Q42" s="6"/>
+    </row>
+    <row r="43" spans="1:17" ht="17">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="6"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="7"/>
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
-    </row>
-    <row r="44" spans="1:16" ht="17">
-      <c r="A44" s="9"/>
+      <c r="Q43" s="6"/>
+    </row>
+    <row r="44" spans="1:17" ht="17">
       <c r="B44" s="9"/>
-      <c r="C44" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="C44" s="9"/>
       <c r="D44" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="6"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="7"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
-    </row>
-    <row r="45" spans="1:16" ht="17">
-      <c r="A45" s="9"/>
+      <c r="Q44" s="6"/>
+    </row>
+    <row r="45" spans="1:17" ht="17">
       <c r="B45" s="9"/>
-      <c r="C45" s="8">
+      <c r="C45" s="9"/>
+      <c r="D45" s="8">
         <v>1</v>
       </c>
-      <c r="D45" s="8">
+      <c r="E45" s="8">
         <v>3</v>
       </c>
-      <c r="E45" s="8">
+      <c r="F45" s="8">
         <v>4</v>
       </c>
-      <c r="F45" s="8">
+      <c r="G45" s="8">
         <v>5</v>
       </c>
-      <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="6"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="7"/>
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
-    </row>
-    <row r="46" spans="1:16" ht="17">
-      <c r="A46" s="9"/>
+      <c r="Q45" s="6"/>
+    </row>
+    <row r="46" spans="1:17" ht="17">
       <c r="B46" s="9"/>
-      <c r="C46" s="8"/>
+      <c r="C46" s="9"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
@@ -1641,169 +1522,175 @@
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="6"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="7"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
-    </row>
-    <row r="47" spans="1:16" ht="17">
-      <c r="A47" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="8"/>
+      <c r="Q46" s="6"/>
+    </row>
+    <row r="47" spans="1:17" ht="17">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="6"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="7"/>
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
-    </row>
-    <row r="48" spans="1:16" ht="17">
-      <c r="A48" s="9"/>
+      <c r="Q47" s="6"/>
+    </row>
+    <row r="48" spans="1:17" ht="17">
       <c r="B48" s="9"/>
-      <c r="C48" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="C48" s="9"/>
       <c r="D48" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="6"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="7"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
-    </row>
-    <row r="49" spans="1:16" ht="17">
-      <c r="A49" s="9"/>
+      <c r="Q48" s="6"/>
+    </row>
+    <row r="49" spans="1:17" ht="17">
       <c r="B49" s="9"/>
-      <c r="C49" s="8">
+      <c r="C49" s="9"/>
+      <c r="D49" s="8">
         <v>5</v>
       </c>
-      <c r="D49" s="8">
+      <c r="E49" s="8">
         <v>1</v>
       </c>
-      <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="6"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="7"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
-    </row>
-    <row r="50" spans="1:16" ht="17">
-      <c r="A50" s="10"/>
+      <c r="Q49" s="6"/>
+    </row>
+    <row r="50" spans="1:17" ht="17">
       <c r="B50" s="10"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="8"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="12"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="6"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="7"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
-    </row>
-    <row r="51" spans="1:16" ht="17">
-      <c r="A51" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D51" s="8"/>
+      <c r="Q50" s="6"/>
+    </row>
+    <row r="51" spans="1:17" ht="17">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="6"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="7"/>
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
-    </row>
-    <row r="52" spans="1:16" ht="17">
-      <c r="A52" s="9"/>
+      <c r="Q51" s="6"/>
+    </row>
+    <row r="52" spans="1:17" ht="17">
       <c r="B52" s="9"/>
-      <c r="C52" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="C52" s="9"/>
       <c r="D52" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F52" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="6"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="7"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
       <c r="P52" s="6"/>
-    </row>
-    <row r="53" spans="1:16" ht="17">
-      <c r="A53" s="9"/>
+      <c r="Q52" s="6"/>
+    </row>
+    <row r="53" spans="1:17" ht="17">
       <c r="B53" s="9"/>
-      <c r="C53" s="8">
+      <c r="C53" s="9"/>
+      <c r="D53" s="8">
         <v>5</v>
       </c>
-      <c r="D53" s="8">
+      <c r="E53" s="8">
         <v>0</v>
       </c>
-      <c r="E53" s="8">
+      <c r="F53" s="8">
         <v>2</v>
       </c>
-      <c r="F53" s="8"/>
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="6"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="7"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
-    </row>
-    <row r="54" spans="1:16" ht="17">
-      <c r="A54" s="9"/>
+      <c r="Q53" s="6"/>
+    </row>
+    <row r="54" spans="1:17" ht="17">
       <c r="B54" s="9"/>
-      <c r="C54" s="8"/>
+      <c r="C54" s="9"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
@@ -1811,82 +1698,70 @@
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="6"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="7"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
-    </row>
-    <row r="55" spans="1:16" ht="17">
-      <c r="A55" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D55" s="8"/>
+      <c r="Q54" s="6"/>
+    </row>
+    <row r="55" spans="1:17" ht="17">
+      <c r="B55" s="9"/>
+      <c r="C55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="6"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="7"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
-    </row>
-    <row r="56" spans="1:16" ht="17">
-      <c r="A56" s="9"/>
+      <c r="Q55" s="6"/>
+    </row>
+    <row r="56" spans="1:17" ht="17">
       <c r="B56" s="9"/>
-      <c r="C56" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="6"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="7"/>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
       <c r="P56" s="6"/>
-    </row>
-    <row r="57" spans="1:16" ht="17">
-      <c r="A57" s="9"/>
+      <c r="Q56" s="6"/>
+    </row>
+    <row r="57" spans="1:17" ht="17">
       <c r="B57" s="9"/>
-      <c r="C57" s="8">
-        <v>6</v>
-      </c>
-      <c r="D57" s="8">
-        <v>0</v>
-      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="6"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="7"/>
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
-    </row>
-    <row r="58" spans="1:16" ht="17">
-      <c r="A58" s="9"/>
+      <c r="Q57" s="6"/>
+    </row>
+    <row r="58" spans="1:17" ht="17">
       <c r="B58" s="9"/>
-      <c r="C58" s="8"/>
+      <c r="C58" s="9"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
@@ -1894,169 +1769,141 @@
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="6"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="7"/>
       <c r="M58" s="6"/>
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
-    </row>
-    <row r="59" spans="1:16" ht="17">
-      <c r="A59" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="8"/>
+      <c r="Q58" s="6"/>
+    </row>
+    <row r="59" spans="1:17" ht="17">
+      <c r="B59" s="9"/>
+      <c r="C59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="6"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="7"/>
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
-    </row>
-    <row r="60" spans="1:16" ht="17">
-      <c r="A60" s="9"/>
+      <c r="Q59" s="6"/>
+    </row>
+    <row r="60" spans="1:17" ht="17">
       <c r="B60" s="9"/>
-      <c r="C60" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="6"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="7"/>
       <c r="M60" s="6"/>
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
       <c r="P60" s="6"/>
-    </row>
-    <row r="61" spans="1:16" ht="17">
-      <c r="A61" s="9"/>
+      <c r="Q60" s="6"/>
+    </row>
+    <row r="61" spans="1:17" ht="17">
       <c r="B61" s="9"/>
-      <c r="C61" s="8">
-        <v>5</v>
-      </c>
-      <c r="D61" s="8">
-        <v>0</v>
-      </c>
-      <c r="E61" s="12">
-        <v>2</v>
-      </c>
-      <c r="F61" s="8"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="12"/>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="6"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="7"/>
       <c r="M61" s="6"/>
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
-    </row>
-    <row r="62" spans="1:16" ht="17">
-      <c r="A62" s="10"/>
+      <c r="Q61" s="6"/>
+    </row>
+    <row r="62" spans="1:17" ht="17">
       <c r="B62" s="10"/>
-      <c r="C62" s="12"/>
+      <c r="C62" s="10"/>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
-      <c r="F62" s="8"/>
+      <c r="F62" s="12"/>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="6"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="7"/>
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
       <c r="P62" s="6"/>
-    </row>
-    <row r="63" spans="1:16" ht="17">
-      <c r="A63" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="8"/>
+      <c r="Q62" s="6"/>
+    </row>
+    <row r="63" spans="1:17" ht="17">
+      <c r="B63" s="9"/>
+      <c r="C63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="12"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="6"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="7"/>
       <c r="M63" s="6"/>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
-    </row>
-    <row r="64" spans="1:16" ht="17">
-      <c r="A64" s="9"/>
+      <c r="Q63" s="6"/>
+    </row>
+    <row r="64" spans="1:17" ht="17">
       <c r="B64" s="9"/>
-      <c r="C64" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E64" s="12"/>
-      <c r="F64" s="8"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="12"/>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="6"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="7"/>
       <c r="M64" s="6"/>
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
       <c r="P64" s="6"/>
-    </row>
-    <row r="65" spans="1:16" ht="17">
-      <c r="A65" s="9"/>
+      <c r="Q64" s="6"/>
+    </row>
+    <row r="65" spans="2:17" ht="17">
       <c r="B65" s="9"/>
-      <c r="C65" s="8">
-        <v>5</v>
-      </c>
-      <c r="D65" s="8">
-        <v>0</v>
-      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
       <c r="I65" s="8"/>
       <c r="J65" s="8"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="6"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="7"/>
       <c r="M65" s="6"/>
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
       <c r="P65" s="6"/>
-    </row>
-    <row r="66" spans="1:16" ht="17">
-      <c r="A66" s="9"/>
+      <c r="Q65" s="6"/>
+    </row>
+    <row r="66" spans="2:17" ht="17">
       <c r="B66" s="9"/>
-      <c r="C66" s="8"/>
+      <c r="C66" s="9"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
@@ -2064,86 +1911,70 @@
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="6"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="7"/>
       <c r="M66" s="6"/>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
       <c r="P66" s="6"/>
-    </row>
-    <row r="67" spans="1:16" ht="17">
-      <c r="A67" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D67" s="8"/>
+      <c r="Q66" s="6"/>
+    </row>
+    <row r="67" spans="2:17" ht="17">
+      <c r="B67" s="9"/>
+      <c r="C67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
       <c r="J67" s="8"/>
-      <c r="K67" s="7"/>
-      <c r="L67" s="6"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="7"/>
       <c r="M67" s="6"/>
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
       <c r="P67" s="6"/>
-    </row>
-    <row r="68" spans="1:16" ht="17">
-      <c r="A68" s="9"/>
+      <c r="Q67" s="6"/>
+    </row>
+    <row r="68" spans="2:17" ht="17">
       <c r="B68" s="9"/>
-      <c r="C68" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="6"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="7"/>
       <c r="M68" s="6"/>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
       <c r="P68" s="6"/>
-    </row>
-    <row r="69" spans="1:16" ht="17">
-      <c r="A69" s="9"/>
+      <c r="Q68" s="6"/>
+    </row>
+    <row r="69" spans="2:17" ht="17">
       <c r="B69" s="9"/>
-      <c r="C69" s="8">
-        <v>5</v>
-      </c>
-      <c r="D69" s="8">
-        <v>0</v>
-      </c>
-      <c r="E69" s="8">
-        <v>2</v>
-      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
       <c r="J69" s="8"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="6"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="7"/>
       <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
       <c r="P69" s="6"/>
-    </row>
-    <row r="70" spans="1:16" ht="17">
-      <c r="A70" s="9"/>
+      <c r="Q69" s="6"/>
+    </row>
+    <row r="70" spans="2:17" ht="17">
       <c r="B70" s="9"/>
-      <c r="C70" s="8"/>
+      <c r="C70" s="9"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
@@ -2151,86 +1982,70 @@
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="8"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="6"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="7"/>
       <c r="M70" s="6"/>
       <c r="N70" s="6"/>
       <c r="O70" s="6"/>
       <c r="P70" s="6"/>
-    </row>
-    <row r="71" spans="1:16" ht="17">
-      <c r="A71" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D71" s="8"/>
+      <c r="Q70" s="6"/>
+    </row>
+    <row r="71" spans="2:17" ht="17">
+      <c r="B71" s="9"/>
+      <c r="C71" s="8"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
       <c r="J71" s="8"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="6"/>
+      <c r="K71" s="8"/>
+      <c r="L71" s="7"/>
       <c r="M71" s="6"/>
       <c r="N71" s="6"/>
       <c r="O71" s="6"/>
       <c r="P71" s="6"/>
-    </row>
-    <row r="72" spans="1:16" ht="17">
-      <c r="A72" s="9"/>
+      <c r="Q71" s="6"/>
+    </row>
+    <row r="72" spans="2:17" ht="17">
       <c r="B72" s="9"/>
-      <c r="C72" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="6"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="7"/>
       <c r="M72" s="6"/>
       <c r="N72" s="6"/>
       <c r="O72" s="6"/>
       <c r="P72" s="6"/>
-    </row>
-    <row r="73" spans="1:16" ht="17">
-      <c r="A73" s="9"/>
+      <c r="Q72" s="6"/>
+    </row>
+    <row r="73" spans="2:17" ht="17">
       <c r="B73" s="9"/>
-      <c r="C73" s="8">
-        <v>7</v>
-      </c>
-      <c r="D73" s="8">
-        <v>0</v>
-      </c>
-      <c r="E73" s="8">
-        <v>3</v>
-      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
       <c r="J73" s="8"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="6"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="7"/>
       <c r="M73" s="6"/>
       <c r="N73" s="6"/>
       <c r="O73" s="6"/>
       <c r="P73" s="6"/>
-    </row>
-    <row r="74" spans="1:16" ht="17">
-      <c r="A74" s="9"/>
+      <c r="Q73" s="6"/>
+    </row>
+    <row r="74" spans="2:17" ht="17">
       <c r="B74" s="9"/>
-      <c r="C74" s="8"/>
+      <c r="C74" s="9"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
@@ -2238,94 +2053,70 @@
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="6"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="7"/>
       <c r="M74" s="6"/>
       <c r="N74" s="6"/>
       <c r="O74" s="6"/>
       <c r="P74" s="6"/>
-    </row>
-    <row r="75" spans="1:16" ht="17">
-      <c r="A75" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D75" s="8"/>
+      <c r="Q74" s="6"/>
+    </row>
+    <row r="75" spans="2:17" ht="17">
+      <c r="B75" s="9"/>
+      <c r="C75" s="8"/>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
       <c r="J75" s="8"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="6"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="7"/>
       <c r="M75" s="6"/>
       <c r="N75" s="6"/>
       <c r="O75" s="6"/>
       <c r="P75" s="6"/>
-    </row>
-    <row r="76" spans="1:16" ht="17">
-      <c r="A76" s="9"/>
+      <c r="Q75" s="6"/>
+    </row>
+    <row r="76" spans="2:17" ht="17">
       <c r="B76" s="9"/>
-      <c r="C76" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
-      <c r="K76" s="7"/>
-      <c r="L76" s="6"/>
+      <c r="K76" s="8"/>
+      <c r="L76" s="7"/>
       <c r="M76" s="6"/>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
       <c r="P76" s="6"/>
-    </row>
-    <row r="77" spans="1:16" ht="17">
-      <c r="A77" s="9"/>
+      <c r="Q76" s="6"/>
+    </row>
+    <row r="77" spans="2:17" ht="17">
       <c r="B77" s="9"/>
-      <c r="C77" s="8">
-        <v>0</v>
-      </c>
-      <c r="D77" s="8">
-        <v>1</v>
-      </c>
-      <c r="E77" s="8">
-        <v>4</v>
-      </c>
-      <c r="F77" s="8">
-        <v>7</v>
-      </c>
-      <c r="G77" s="8">
-        <v>1</v>
-      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
       <c r="J77" s="8"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="6"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="7"/>
       <c r="M77" s="6"/>
       <c r="N77" s="6"/>
       <c r="O77" s="6"/>
       <c r="P77" s="6"/>
-    </row>
-    <row r="78" spans="1:16" ht="17">
-      <c r="A78" s="9"/>
+      <c r="Q77" s="6"/>
+    </row>
+    <row r="78" spans="2:17" ht="17">
       <c r="B78" s="9"/>
-      <c r="C78" s="8"/>
+      <c r="C78" s="9"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
@@ -2333,98 +2124,70 @@
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="6"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="7"/>
       <c r="M78" s="6"/>
       <c r="N78" s="6"/>
       <c r="O78" s="6"/>
       <c r="P78" s="6"/>
-    </row>
-    <row r="79" spans="1:16" ht="17">
-      <c r="A79" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D79" s="8"/>
+      <c r="Q78" s="6"/>
+    </row>
+    <row r="79" spans="2:17" ht="17">
+      <c r="B79" s="9"/>
+      <c r="C79" s="8"/>
       <c r="E79" s="8"/>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
       <c r="J79" s="8"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="6"/>
+      <c r="K79" s="8"/>
+      <c r="L79" s="7"/>
       <c r="M79" s="6"/>
       <c r="N79" s="6"/>
       <c r="O79" s="6"/>
       <c r="P79" s="6"/>
-    </row>
-    <row r="80" spans="1:16" ht="17">
-      <c r="A80" s="9"/>
+      <c r="Q79" s="6"/>
+    </row>
+    <row r="80" spans="2:17" ht="17">
       <c r="B80" s="9"/>
-      <c r="C80" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F80" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H80" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
       <c r="I80" s="8"/>
       <c r="J80" s="8"/>
-      <c r="K80" s="7"/>
-      <c r="L80" s="6"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="7"/>
       <c r="M80" s="6"/>
       <c r="N80" s="6"/>
       <c r="O80" s="6"/>
       <c r="P80" s="6"/>
-    </row>
-    <row r="81" spans="1:16" ht="17">
-      <c r="A81" s="9"/>
+      <c r="Q80" s="6"/>
+    </row>
+    <row r="81" spans="2:17" ht="17">
       <c r="B81" s="9"/>
-      <c r="C81" s="8">
-        <v>0</v>
-      </c>
-      <c r="D81" s="8">
-        <v>8</v>
-      </c>
-      <c r="E81" s="8">
-        <v>5</v>
-      </c>
-      <c r="F81" s="8">
-        <v>3</v>
-      </c>
-      <c r="G81" s="8">
-        <v>1</v>
-      </c>
-      <c r="H81" s="8">
-        <v>3</v>
-      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="6"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="7"/>
       <c r="M81" s="6"/>
       <c r="N81" s="6"/>
       <c r="O81" s="6"/>
       <c r="P81" s="6"/>
-    </row>
-    <row r="82" spans="1:16" ht="17">
-      <c r="A82" s="9"/>
+      <c r="Q81" s="6"/>
+    </row>
+    <row r="82" spans="2:17" ht="17">
       <c r="B82" s="9"/>
-      <c r="C82" s="8"/>
+      <c r="C82" s="9"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
@@ -2432,20 +2195,16 @@
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
-      <c r="K82" s="7"/>
-      <c r="L82" s="6"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="7"/>
       <c r="M82" s="6"/>
       <c r="N82" s="6"/>
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
-    </row>
-    <row r="83" spans="1:16" ht="17">
-      <c r="A83" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>78</v>
-      </c>
+      <c r="Q82" s="6"/>
+    </row>
+    <row r="83" spans="2:17" ht="17">
+      <c r="B83" s="9"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
@@ -2454,19 +2213,17 @@
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
-      <c r="K83" s="7"/>
-      <c r="L83" s="6"/>
+      <c r="K83" s="8"/>
+      <c r="L83" s="7"/>
       <c r="M83" s="6"/>
       <c r="N83" s="6"/>
       <c r="O83" s="6"/>
       <c r="P83" s="6"/>
-    </row>
-    <row r="84" spans="1:16" ht="17">
-      <c r="A84" s="9"/>
+      <c r="Q83" s="6"/>
+    </row>
+    <row r="84" spans="2:17" ht="17">
       <c r="B84" s="9"/>
-      <c r="C84" s="8" t="s">
-        <v>88</v>
-      </c>
+      <c r="C84" s="9"/>
       <c r="D84" s="8"/>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
@@ -2474,17 +2231,17 @@
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
-      <c r="K84" s="7"/>
-      <c r="L84" s="6"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="7"/>
       <c r="M84" s="6"/>
       <c r="N84" s="6"/>
       <c r="O84" s="6"/>
       <c r="P84" s="6"/>
-    </row>
-    <row r="85" spans="1:16" ht="17">
-      <c r="A85" s="9"/>
+      <c r="Q84" s="6"/>
+    </row>
+    <row r="85" spans="2:17" ht="17">
       <c r="B85" s="9"/>
-      <c r="C85" s="8"/>
+      <c r="C85" s="9"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
       <c r="F85" s="8"/>
@@ -2492,17 +2249,17 @@
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
-      <c r="K85" s="7"/>
-      <c r="L85" s="6"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="7"/>
       <c r="M85" s="6"/>
       <c r="N85" s="6"/>
       <c r="O85" s="6"/>
       <c r="P85" s="6"/>
-    </row>
-    <row r="86" spans="1:16" ht="17">
-      <c r="A86" s="9"/>
+      <c r="Q85" s="6"/>
+    </row>
+    <row r="86" spans="2:17" ht="17">
       <c r="B86" s="9"/>
-      <c r="C86" s="8"/>
+      <c r="C86" s="9"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
       <c r="F86" s="8"/>
@@ -2510,17 +2267,17 @@
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
-      <c r="K86" s="7"/>
-      <c r="L86" s="6"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="7"/>
       <c r="M86" s="6"/>
       <c r="N86" s="6"/>
       <c r="O86" s="6"/>
       <c r="P86" s="6"/>
-    </row>
-    <row r="87" spans="1:16" ht="17">
-      <c r="A87" s="9"/>
+      <c r="Q86" s="6"/>
+    </row>
+    <row r="87" spans="2:17" ht="17">
       <c r="B87" s="9"/>
-      <c r="C87" s="8"/>
+      <c r="C87" s="9"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
       <c r="F87" s="8"/>
@@ -2528,17 +2285,17 @@
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="6"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="7"/>
       <c r="M87" s="6"/>
       <c r="N87" s="6"/>
       <c r="O87" s="6"/>
       <c r="P87" s="6"/>
-    </row>
-    <row r="88" spans="1:16" ht="17">
-      <c r="A88" s="9"/>
+      <c r="Q87" s="6"/>
+    </row>
+    <row r="88" spans="2:17" ht="17">
       <c r="B88" s="9"/>
-      <c r="C88" s="8"/>
+      <c r="C88" s="9"/>
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
       <c r="F88" s="8"/>
@@ -2546,17 +2303,17 @@
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
       <c r="J88" s="8"/>
-      <c r="K88" s="7"/>
-      <c r="L88" s="6"/>
+      <c r="K88" s="8"/>
+      <c r="L88" s="7"/>
       <c r="M88" s="6"/>
       <c r="N88" s="6"/>
       <c r="O88" s="6"/>
       <c r="P88" s="6"/>
-    </row>
-    <row r="89" spans="1:16" ht="17">
-      <c r="A89" s="9"/>
+      <c r="Q88" s="6"/>
+    </row>
+    <row r="89" spans="2:17" ht="17">
       <c r="B89" s="9"/>
-      <c r="C89" s="8"/>
+      <c r="C89" s="9"/>
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
@@ -2564,335 +2321,281 @@
       <c r="H89" s="8"/>
       <c r="I89" s="8"/>
       <c r="J89" s="8"/>
-      <c r="K89" s="7"/>
-      <c r="L89" s="6"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="7"/>
       <c r="M89" s="6"/>
       <c r="N89" s="6"/>
       <c r="O89" s="6"/>
       <c r="P89" s="6"/>
-    </row>
-    <row r="90" spans="1:16" ht="17">
-      <c r="A90" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D90" s="12"/>
+      <c r="Q89" s="6"/>
+    </row>
+    <row r="90" spans="2:17" ht="17">
+      <c r="B90" s="10"/>
+      <c r="C90" s="12"/>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
-      <c r="I90" s="7"/>
+      <c r="I90" s="12"/>
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
-      <c r="L90" s="6"/>
+      <c r="L90" s="7"/>
       <c r="M90" s="6"/>
       <c r="N90" s="6"/>
       <c r="O90" s="6"/>
       <c r="P90" s="6"/>
-    </row>
-    <row r="91" spans="1:16" ht="17">
-      <c r="A91" s="10"/>
+      <c r="Q90" s="6"/>
+    </row>
+    <row r="91" spans="2:17" ht="17">
       <c r="B91" s="10"/>
-      <c r="C91" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E91" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F91" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="C91" s="10"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
-      <c r="I91" s="7"/>
+      <c r="I91" s="12"/>
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
-      <c r="L91" s="6"/>
+      <c r="L91" s="7"/>
       <c r="M91" s="6"/>
       <c r="N91" s="6"/>
       <c r="O91" s="6"/>
       <c r="P91" s="6"/>
-    </row>
-    <row r="92" spans="1:16" ht="17">
-      <c r="A92" s="10"/>
+      <c r="Q91" s="6"/>
+    </row>
+    <row r="92" spans="2:17" ht="17">
       <c r="B92" s="10"/>
-      <c r="C92" s="12">
-        <v>7</v>
-      </c>
-      <c r="D92" s="12">
-        <v>5</v>
-      </c>
-      <c r="E92" s="12">
-        <v>3</v>
-      </c>
-      <c r="F92" s="12">
-        <v>1</v>
-      </c>
+      <c r="C92" s="10"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
-      <c r="I92" s="7"/>
+      <c r="I92" s="12"/>
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
-      <c r="L92" s="6"/>
+      <c r="L92" s="7"/>
       <c r="M92" s="6"/>
       <c r="N92" s="6"/>
       <c r="O92" s="6"/>
       <c r="P92" s="6"/>
-    </row>
-    <row r="93" spans="1:16" ht="17">
-      <c r="A93" s="10"/>
+      <c r="Q92" s="6"/>
+    </row>
+    <row r="93" spans="2:17" ht="17">
       <c r="B93" s="10"/>
-      <c r="C93" s="12"/>
+      <c r="C93" s="10"/>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
-      <c r="I93" s="7"/>
+      <c r="I93" s="12"/>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
-      <c r="L93" s="6"/>
+      <c r="L93" s="7"/>
       <c r="M93" s="6"/>
       <c r="N93" s="6"/>
       <c r="O93" s="6"/>
       <c r="P93" s="6"/>
-    </row>
-    <row r="94" spans="1:16" ht="17">
-      <c r="A94" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B94" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D94" s="12"/>
+      <c r="Q93" s="6"/>
+    </row>
+    <row r="94" spans="2:17" ht="17">
+      <c r="B94" s="10"/>
+      <c r="C94" s="12"/>
       <c r="E94" s="12"/>
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="7"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="5"/>
       <c r="K94" s="7"/>
-      <c r="L94" s="6"/>
+      <c r="L94" s="7"/>
       <c r="M94" s="6"/>
       <c r="N94" s="6"/>
       <c r="O94" s="6"/>
       <c r="P94" s="6"/>
-    </row>
-    <row r="95" spans="1:16" ht="17">
-      <c r="A95" s="10"/>
+      <c r="Q94" s="6"/>
+    </row>
+    <row r="95" spans="2:17" ht="17">
       <c r="B95" s="10"/>
-      <c r="C95" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D95" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F95" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G95" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H95" s="13"/>
-      <c r="I95" s="5"/>
-      <c r="J95" s="7"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="5"/>
       <c r="K95" s="7"/>
-      <c r="L95" s="6"/>
+      <c r="L95" s="7"/>
       <c r="M95" s="6"/>
       <c r="N95" s="6"/>
       <c r="O95" s="6"/>
       <c r="P95" s="6"/>
-    </row>
-    <row r="96" spans="1:16" ht="17">
-      <c r="A96" s="10"/>
+      <c r="Q95" s="6"/>
+    </row>
+    <row r="96" spans="2:17" ht="17">
       <c r="B96" s="10"/>
-      <c r="C96" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D96" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E96" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F96" s="12" t="s">
-        <v>66</v>
-      </c>
+      <c r="C96" s="10"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
       <c r="G96" s="12"/>
-      <c r="H96" s="13"/>
-      <c r="I96" s="5"/>
-      <c r="J96" s="7"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="5"/>
       <c r="K96" s="7"/>
-      <c r="L96" s="6"/>
+      <c r="L96" s="7"/>
       <c r="M96" s="6"/>
       <c r="N96" s="6"/>
       <c r="O96" s="6"/>
       <c r="P96" s="6"/>
-    </row>
-    <row r="97" spans="1:16" ht="17">
-      <c r="A97" s="10"/>
+      <c r="Q96" s="6"/>
+    </row>
+    <row r="97" spans="2:17" ht="17">
       <c r="B97" s="10"/>
-      <c r="C97" s="12"/>
+      <c r="C97" s="10"/>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
       <c r="F97" s="12"/>
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
-      <c r="I97" s="7"/>
+      <c r="I97" s="12"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
-      <c r="L97" s="6"/>
+      <c r="L97" s="7"/>
       <c r="M97" s="6"/>
       <c r="N97" s="6"/>
       <c r="O97" s="6"/>
       <c r="P97" s="6"/>
-    </row>
-    <row r="98" spans="1:16" ht="17">
-      <c r="A98" s="10"/>
+      <c r="Q97" s="6"/>
+    </row>
+    <row r="98" spans="2:17" ht="17">
       <c r="B98" s="10"/>
-      <c r="C98" s="12"/>
+      <c r="C98" s="10"/>
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
       <c r="F98" s="12"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
-      <c r="I98" s="7"/>
+      <c r="I98" s="12"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
-      <c r="L98" s="6"/>
+      <c r="L98" s="7"/>
       <c r="M98" s="6"/>
       <c r="N98" s="6"/>
       <c r="O98" s="6"/>
       <c r="P98" s="6"/>
-    </row>
-    <row r="99" spans="1:16" ht="17">
-      <c r="A99" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B99" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D99" s="12"/>
+      <c r="Q98" s="6"/>
+    </row>
+    <row r="99" spans="2:17" ht="17">
+      <c r="B99" s="10"/>
+      <c r="C99" s="12"/>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
-      <c r="I99" s="7"/>
+      <c r="I99" s="12"/>
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
-      <c r="L99" s="6"/>
+      <c r="L99" s="7"/>
       <c r="M99" s="6"/>
       <c r="N99" s="6"/>
       <c r="O99" s="6"/>
       <c r="P99" s="6"/>
-    </row>
-    <row r="100" spans="1:16" ht="17">
-      <c r="A100" s="10"/>
+      <c r="Q99" s="6"/>
+    </row>
+    <row r="100" spans="2:17" ht="17">
       <c r="B100" s="10"/>
-      <c r="C100" s="12" t="s">
-        <v>68</v>
-      </c>
+      <c r="C100" s="10"/>
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
-      <c r="I100" s="7"/>
+      <c r="I100" s="12"/>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
-      <c r="L100" s="6"/>
+      <c r="L100" s="7"/>
       <c r="M100" s="6"/>
       <c r="N100" s="6"/>
       <c r="O100" s="6"/>
       <c r="P100" s="6"/>
-    </row>
-    <row r="101" spans="1:16" ht="17">
-      <c r="A101" s="10"/>
+      <c r="Q100" s="6"/>
+    </row>
+    <row r="101" spans="2:17" ht="17">
       <c r="B101" s="10"/>
-      <c r="C101" s="12"/>
+      <c r="C101" s="10"/>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
       <c r="F101" s="12"/>
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
-      <c r="I101" s="7"/>
+      <c r="I101" s="12"/>
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
-      <c r="L101" s="6"/>
+      <c r="L101" s="7"/>
       <c r="M101" s="6"/>
       <c r="N101" s="6"/>
       <c r="O101" s="6"/>
       <c r="P101" s="6"/>
-    </row>
-    <row r="102" spans="1:16" ht="17">
-      <c r="A102" s="10"/>
+      <c r="Q101" s="6"/>
+    </row>
+    <row r="102" spans="2:17" ht="17">
       <c r="B102" s="10"/>
-      <c r="C102" s="12"/>
+      <c r="C102" s="10"/>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
-      <c r="I102" s="7"/>
+      <c r="I102" s="12"/>
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
-      <c r="L102" s="6"/>
+      <c r="L102" s="7"/>
       <c r="M102" s="6"/>
       <c r="N102" s="6"/>
       <c r="O102" s="6"/>
       <c r="P102" s="6"/>
-    </row>
-    <row r="103" spans="1:16" ht="17">
-      <c r="A103" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B103" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D103" s="12"/>
+      <c r="Q102" s="6"/>
+    </row>
+    <row r="103" spans="2:17" ht="17">
+      <c r="B103" s="10"/>
+      <c r="C103" s="12"/>
       <c r="E103" s="12"/>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
-      <c r="I103" s="7"/>
+      <c r="I103" s="12"/>
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
-      <c r="L103" s="6"/>
+      <c r="L103" s="7"/>
       <c r="M103" s="6"/>
       <c r="N103" s="6"/>
       <c r="O103" s="6"/>
       <c r="P103" s="6"/>
-    </row>
-    <row r="104" spans="1:16" ht="17">
-      <c r="A104" s="10"/>
+      <c r="Q103" s="6"/>
+    </row>
+    <row r="104" spans="2:17" ht="17">
       <c r="B104" s="10"/>
-      <c r="C104" s="12" t="s">
-        <v>70</v>
-      </c>
+      <c r="C104" s="10"/>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
-      <c r="I104" s="7"/>
+      <c r="I104" s="12"/>
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
-      <c r="L104" s="6"/>
+      <c r="L104" s="7"/>
       <c r="M104" s="6"/>
       <c r="N104" s="6"/>
       <c r="O104" s="6"/>
       <c r="P104" s="6"/>
-    </row>
-    <row r="105" spans="1:16">
-      <c r="A105" s="11"/>
+      <c r="Q104" s="6"/>
+    </row>
+    <row r="105" spans="2:17">
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
@@ -2903,9 +2606,9 @@
       <c r="I105" s="11"/>
       <c r="J105" s="11"/>
       <c r="K105" s="11"/>
-    </row>
-    <row r="106" spans="1:16">
-      <c r="A106" s="11"/>
+      <c r="L105" s="11"/>
+    </row>
+    <row r="106" spans="2:17">
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
@@ -2916,9 +2619,9 @@
       <c r="I106" s="11"/>
       <c r="J106" s="11"/>
       <c r="K106" s="11"/>
-    </row>
-    <row r="107" spans="1:16">
-      <c r="A107" s="11"/>
+      <c r="L106" s="11"/>
+    </row>
+    <row r="107" spans="2:17">
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
@@ -2929,9 +2632,9 @@
       <c r="I107" s="11"/>
       <c r="J107" s="11"/>
       <c r="K107" s="11"/>
-    </row>
-    <row r="108" spans="1:16">
-      <c r="A108" s="11"/>
+      <c r="L107" s="11"/>
+    </row>
+    <row r="108" spans="2:17">
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
@@ -2942,9 +2645,9 @@
       <c r="I108" s="11"/>
       <c r="J108" s="11"/>
       <c r="K108" s="11"/>
-    </row>
-    <row r="109" spans="1:16">
-      <c r="A109" s="11"/>
+      <c r="L108" s="11"/>
+    </row>
+    <row r="109" spans="2:17">
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
@@ -2955,9 +2658,9 @@
       <c r="I109" s="11"/>
       <c r="J109" s="11"/>
       <c r="K109" s="11"/>
-    </row>
-    <row r="110" spans="1:16">
-      <c r="A110" s="11"/>
+      <c r="L109" s="11"/>
+    </row>
+    <row r="110" spans="2:17">
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
@@ -2968,9 +2671,9 @@
       <c r="I110" s="11"/>
       <c r="J110" s="11"/>
       <c r="K110" s="11"/>
-    </row>
-    <row r="111" spans="1:16">
-      <c r="A111" s="11"/>
+      <c r="L110" s="11"/>
+    </row>
+    <row r="111" spans="2:17">
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
@@ -2981,6 +2684,7 @@
       <c r="I111" s="11"/>
       <c r="J111" s="11"/>
       <c r="K111" s="11"/>
+      <c r="L111" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed the new PieChart page
</commit_message>
<xml_diff>
--- a/Python/src/_Highlands/questions.xlsx
+++ b/Python/src/_Highlands/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
   <si>
     <t>Question</t>
   </si>
@@ -81,6 +81,12 @@
     <t>text</t>
   </si>
   <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
     <t>Once a half year or less</t>
   </si>
   <si>
@@ -105,6 +111,81 @@
     <t>I do know at this time</t>
   </si>
   <si>
+    <t>Do not know</t>
+  </si>
+  <si>
+    <t>Does not meet</t>
+  </si>
+  <si>
+    <t>1 to 3</t>
+  </si>
+  <si>
+    <t>3 to 5</t>
+  </si>
+  <si>
+    <t>More than 5 times a year</t>
+  </si>
+  <si>
+    <t>I do not know</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>Annually</t>
+  </si>
+  <si>
+    <t>The client sells services / consulting</t>
+  </si>
+  <si>
+    <t>The client sells products</t>
+  </si>
+  <si>
+    <t>The client sells both services and products</t>
+  </si>
+  <si>
+    <t>The client is a non profit organization</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>Last 30 days</t>
+  </si>
+  <si>
+    <t>Last 90 days</t>
+  </si>
+  <si>
+    <t>Last 180 days</t>
+  </si>
+  <si>
+    <t>In the past year</t>
+  </si>
+  <si>
+    <t>Extremely serious</t>
+  </si>
+  <si>
+    <t>Significant but quickly resolved</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Please describe the business impact in terms of how it will impact key business measurements of importance to their board.</t>
+  </si>
+  <si>
+    <t>Please enter "X,Y"  (X = Market Growth), Y = Client Revenue Growth): Major Decline = 0, Flat = 5, Very Strong = 10</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -135,6 +216,30 @@
     <t>This is the Highlands Client Teaming Assessment.  It will help establish the likelihood of a Sales Trinity being created and then delivering a True Business Solution.   Version Draft2.3</t>
   </si>
   <si>
+    <t>What Client are you assessing?</t>
+  </si>
+  <si>
+    <t>At the end of this questionnaire you will be asked if you want to complete a new form, allowing you to profile another client.</t>
+  </si>
+  <si>
+    <t>Name of client to profile</t>
+  </si>
+  <si>
+    <t>Client location</t>
+  </si>
+  <si>
+    <t>Exploring Relationships</t>
+  </si>
+  <si>
+    <t>This series of questions explores the relationships between you, your "competitor" and the client. These questions help to quantify who knows who and the level of trust and confidence that exists in those relationships.</t>
+  </si>
+  <si>
+    <t>Business Situation</t>
+  </si>
+  <si>
+    <t>This section contains a series of questions to understand the business dynamics of your client</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -144,19 +249,52 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Again, with reference to 8, does your client see the value and want to do this?</t>
+    <t>Thinking as the CEO of your client, what will they say about their relationship with your company?</t>
+  </si>
+  <si>
+    <t>As you think of the business relationship with your client, which of the following best describes the time you spend with them discussing their business?</t>
   </si>
   <si>
     <t>What is your understanding of how your client would react to you working with their other suppliers (that you may commonly refer to as a "competitor") to help them (the client) with their business?</t>
   </si>
   <si>
-    <t>As you think of the business relationship with your client, which of the following best describes the time you spend with them discussing their business?</t>
-  </si>
-  <si>
-    <t>Thinking as the CEO of your client, what will they say about their relationship with your company?</t>
-  </si>
-  <si>
-    <t>Considering your response to 8, do you know why they would say that?</t>
+    <t>Thinking like the client, and reflecting on your responses to Q3a to Q3c, do you understand the benefits to your client?</t>
+  </si>
+  <si>
+    <t>Looking at your answers from Q3a to Q3d inclusive, would your 1st or 2nd line manager agree with you?</t>
+  </si>
+  <si>
+    <t>Has your 1st line or 2nd line manager agreed with you in real time as you answered?</t>
+  </si>
+  <si>
+    <t>Is there a board member in your company that is or would be, an executive sponsor for this type of relationship?</t>
+  </si>
+  <si>
+    <t>How many times a year does your executive sponsor meet with your "competitor"?</t>
+  </si>
+  <si>
+    <t>How often does your sponsor talk informally with their counterpart in your "competitor"?</t>
+  </si>
+  <si>
+    <t>What does your client sell today, that drives most of their sales?</t>
+  </si>
+  <si>
+    <t>Thinking about your company's overall credibility &amp; trust,  have there been any issues that have affected this in the past 12 month or more recently?</t>
+  </si>
+  <si>
+    <t>Thinking like your client, what new business outcomes do they need to obtain to grow their business?</t>
+  </si>
+  <si>
+    <t>Where is your client's business dynamic vs the market dynamic?</t>
+  </si>
+  <si>
+    <t>Considering your response to 10, do you know why they would say that?</t>
+  </si>
+  <si>
+    <t>Again, with reference to 10, does your client see the value and want to do this?</t>
+  </si>
+  <si>
+    <t>If 16 was answered "No", does the sponsor or potential sponsor report to your board?</t>
   </si>
 </sst>
 </file>
@@ -889,24 +1027,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
     <col min="2" max="14" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23">
       <c r="A1" s="4" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -958,10 +1097,10 @@
     </row>
     <row r="4" spans="1:12" ht="17">
       <c r="B4" s="18" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="D4" s="16"/>
       <c r="K4" s="1"/>
@@ -971,7 +1110,7 @@
       <c r="B5" s="18"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -995,13 +1134,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1010,7 +1149,7 @@
       <c r="B9" s="18"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1027,13 +1166,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1042,7 +1181,7 @@
       <c r="B12" s="18"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1059,13 +1198,13 @@
         <v>3</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1074,7 +1213,7 @@
       <c r="B15" s="18"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1091,13 +1230,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1106,7 +1245,7 @@
       <c r="B18" s="18"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1123,13 +1262,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1138,7 +1277,7 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1151,8 +1290,12 @@
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="17">
-      <c r="B23" s="18"/>
-      <c r="C23" s="16"/>
+      <c r="B23" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>62</v>
+      </c>
       <c r="D23" s="16"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1160,7 +1303,9 @@
     <row r="24" spans="1:12">
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="D24" s="16" t="s">
+        <v>66</v>
+      </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
@@ -1172,8 +1317,15 @@
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="17">
-      <c r="B26" s="18"/>
-      <c r="C26" s="16"/>
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="D26" s="16"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1181,7 +1333,9 @@
     <row r="27" spans="1:12" ht="17">
       <c r="B27" s="18"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="D27" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
@@ -1193,8 +1347,15 @@
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="17">
-      <c r="B29" s="18"/>
-      <c r="C29" s="16"/>
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="D29" s="16"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1202,7 +1363,9 @@
     <row r="30" spans="1:12">
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
+      <c r="D30" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
@@ -1212,8 +1375,12 @@
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="17">
-      <c r="B32" s="18"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>62</v>
+      </c>
       <c r="D32" s="16"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1221,7 +1388,9 @@
     <row r="33" spans="1:17" ht="16">
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="19"/>
+      <c r="D33" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
       <c r="G33" s="13"/>
@@ -1246,10 +1415,10 @@
     </row>
     <row r="35" spans="1:17" ht="17">
       <c r="A35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>18</v>
@@ -1336,10 +1505,10 @@
     </row>
     <row r="39" spans="1:17" ht="17">
       <c r="A39">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>18</v>
@@ -1377,7 +1546,7 @@
         <v>14</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
@@ -1438,10 +1607,10 @@
     </row>
     <row r="43" spans="1:17" ht="17">
       <c r="A43">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>18</v>
@@ -1464,16 +1633,16 @@
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
@@ -1532,10 +1701,10 @@
     </row>
     <row r="47" spans="1:17" ht="17">
       <c r="A47">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>18</v>
@@ -1558,10 +1727,10 @@
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
@@ -1618,10 +1787,10 @@
     </row>
     <row r="51" spans="1:17" ht="17">
       <c r="A51">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>18</v>
@@ -1644,13 +1813,13 @@
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
@@ -1707,8 +1876,15 @@
       <c r="Q54" s="6"/>
     </row>
     <row r="55" spans="1:17" ht="17">
-      <c r="B55" s="9"/>
-      <c r="C55" s="8"/>
+      <c r="A55">
+        <v>13</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
@@ -1726,8 +1902,12 @@
     <row r="56" spans="1:17" ht="17">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+      <c r="D56" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
@@ -1744,8 +1924,12 @@
     <row r="57" spans="1:17" ht="17">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
+      <c r="D57" s="8">
+        <v>6</v>
+      </c>
+      <c r="E57" s="8">
+        <v>0</v>
+      </c>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
@@ -1778,8 +1962,15 @@
       <c r="Q58" s="6"/>
     </row>
     <row r="59" spans="1:17" ht="17">
-      <c r="B59" s="9"/>
-      <c r="C59" s="8"/>
+      <c r="A59">
+        <v>14</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
@@ -1797,9 +1988,15 @@
     <row r="60" spans="1:17" ht="17">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
+      <c r="D60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
@@ -1815,9 +2012,15 @@
     <row r="61" spans="1:17" ht="17">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="12"/>
+      <c r="D61" s="8">
+        <v>5</v>
+      </c>
+      <c r="E61" s="8">
+        <v>0</v>
+      </c>
+      <c r="F61" s="12">
+        <v>2</v>
+      </c>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
@@ -1849,8 +2052,15 @@
       <c r="Q62" s="6"/>
     </row>
     <row r="63" spans="1:17" ht="17">
-      <c r="B63" s="9"/>
-      <c r="C63" s="8"/>
+      <c r="A63">
+        <v>15</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E63" s="8"/>
       <c r="F63" s="12"/>
       <c r="G63" s="8"/>
@@ -1868,8 +2078,12 @@
     <row r="64" spans="1:17" ht="17">
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
+      <c r="D64" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="F64" s="12"/>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
@@ -1883,11 +2097,15 @@
       <c r="P64" s="6"/>
       <c r="Q64" s="6"/>
     </row>
-    <row r="65" spans="2:17" ht="17">
+    <row r="65" spans="1:17" ht="17">
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
+      <c r="D65" s="8">
+        <v>5</v>
+      </c>
+      <c r="E65" s="8">
+        <v>0</v>
+      </c>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
@@ -1901,7 +2119,7 @@
       <c r="P65" s="6"/>
       <c r="Q65" s="6"/>
     </row>
-    <row r="66" spans="2:17" ht="17">
+    <row r="66" spans="1:17" ht="17">
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="8"/>
@@ -1919,9 +2137,16 @@
       <c r="P66" s="6"/>
       <c r="Q66" s="6"/>
     </row>
-    <row r="67" spans="2:17" ht="17">
-      <c r="B67" s="9"/>
-      <c r="C67" s="8"/>
+    <row r="67" spans="1:17" ht="17">
+      <c r="A67">
+        <v>16</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
@@ -1936,12 +2161,18 @@
       <c r="P67" s="6"/>
       <c r="Q67" s="6"/>
     </row>
-    <row r="68" spans="2:17" ht="17">
+    <row r="68" spans="1:17" ht="17">
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
+      <c r="D68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
@@ -1954,12 +2185,18 @@
       <c r="P68" s="6"/>
       <c r="Q68" s="6"/>
     </row>
-    <row r="69" spans="2:17" ht="17">
+    <row r="69" spans="1:17" ht="17">
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
+      <c r="D69" s="8">
+        <v>5</v>
+      </c>
+      <c r="E69" s="8">
+        <v>0</v>
+      </c>
+      <c r="F69" s="8">
+        <v>2</v>
+      </c>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
@@ -1972,7 +2209,7 @@
       <c r="P69" s="6"/>
       <c r="Q69" s="6"/>
     </row>
-    <row r="70" spans="2:17" ht="17">
+    <row r="70" spans="1:17" ht="17">
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="8"/>
@@ -1990,9 +2227,16 @@
       <c r="P70" s="6"/>
       <c r="Q70" s="6"/>
     </row>
-    <row r="71" spans="2:17" ht="17">
-      <c r="B71" s="9"/>
-      <c r="C71" s="8"/>
+    <row r="71" spans="1:17" ht="17">
+      <c r="A71">
+        <v>17</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
@@ -2007,12 +2251,18 @@
       <c r="P71" s="6"/>
       <c r="Q71" s="6"/>
     </row>
-    <row r="72" spans="2:17" ht="17">
+    <row r="72" spans="1:17" ht="17">
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
+      <c r="D72" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
@@ -2025,12 +2275,18 @@
       <c r="P72" s="6"/>
       <c r="Q72" s="6"/>
     </row>
-    <row r="73" spans="2:17" ht="17">
+    <row r="73" spans="1:17" ht="17">
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
+      <c r="D73" s="8">
+        <v>7</v>
+      </c>
+      <c r="E73" s="8">
+        <v>0</v>
+      </c>
+      <c r="F73" s="8">
+        <v>3</v>
+      </c>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
@@ -2043,7 +2299,7 @@
       <c r="P73" s="6"/>
       <c r="Q73" s="6"/>
     </row>
-    <row r="74" spans="2:17" ht="17">
+    <row r="74" spans="1:17" ht="17">
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="8"/>
@@ -2061,9 +2317,16 @@
       <c r="P74" s="6"/>
       <c r="Q74" s="6"/>
     </row>
-    <row r="75" spans="2:17" ht="17">
-      <c r="B75" s="9"/>
-      <c r="C75" s="8"/>
+    <row r="75" spans="1:17" ht="17">
+      <c r="A75">
+        <v>18</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
@@ -2078,14 +2341,24 @@
       <c r="P75" s="6"/>
       <c r="Q75" s="6"/>
     </row>
-    <row r="76" spans="2:17" ht="17">
+    <row r="76" spans="1:17" ht="17">
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
+      <c r="D76" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H76" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
@@ -2096,14 +2369,24 @@
       <c r="P76" s="6"/>
       <c r="Q76" s="6"/>
     </row>
-    <row r="77" spans="2:17" ht="17">
+    <row r="77" spans="1:17" ht="17">
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
+      <c r="D77" s="8">
+        <v>0</v>
+      </c>
+      <c r="E77" s="8">
+        <v>1</v>
+      </c>
+      <c r="F77" s="8">
+        <v>4</v>
+      </c>
+      <c r="G77" s="8">
+        <v>7</v>
+      </c>
+      <c r="H77" s="8">
+        <v>1</v>
+      </c>
       <c r="I77" s="8"/>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
@@ -2114,7 +2397,7 @@
       <c r="P77" s="6"/>
       <c r="Q77" s="6"/>
     </row>
-    <row r="78" spans="2:17" ht="17">
+    <row r="78" spans="1:17" ht="17">
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="8"/>
@@ -2132,9 +2415,16 @@
       <c r="P78" s="6"/>
       <c r="Q78" s="6"/>
     </row>
-    <row r="79" spans="2:17" ht="17">
-      <c r="B79" s="9"/>
-      <c r="C79" s="8"/>
+    <row r="79" spans="1:17" ht="17">
+      <c r="A79">
+        <v>19</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E79" s="8"/>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
@@ -2149,15 +2439,27 @@
       <c r="P79" s="6"/>
       <c r="Q79" s="6"/>
     </row>
-    <row r="80" spans="2:17" ht="17">
+    <row r="80" spans="1:17" ht="17">
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
+      <c r="D80" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H80" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I80" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J80" s="8"/>
       <c r="K80" s="8"/>
       <c r="L80" s="7"/>
@@ -2167,15 +2469,27 @@
       <c r="P80" s="6"/>
       <c r="Q80" s="6"/>
     </row>
-    <row r="81" spans="2:17" ht="17">
+    <row r="81" spans="1:17" ht="17">
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
+      <c r="D81" s="8">
+        <v>0</v>
+      </c>
+      <c r="E81" s="8">
+        <v>8</v>
+      </c>
+      <c r="F81" s="8">
+        <v>5</v>
+      </c>
+      <c r="G81" s="8">
+        <v>3</v>
+      </c>
+      <c r="H81" s="8">
+        <v>1</v>
+      </c>
+      <c r="I81" s="8">
+        <v>3</v>
+      </c>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
       <c r="L81" s="7"/>
@@ -2185,7 +2499,7 @@
       <c r="P81" s="6"/>
       <c r="Q81" s="6"/>
     </row>
-    <row r="82" spans="2:17" ht="17">
+    <row r="82" spans="1:17" ht="17">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="8"/>
@@ -2203,9 +2517,13 @@
       <c r="P82" s="6"/>
       <c r="Q82" s="6"/>
     </row>
-    <row r="83" spans="2:17" ht="17">
-      <c r="B83" s="9"/>
-      <c r="C83" s="8"/>
+    <row r="83" spans="1:17" ht="17">
+      <c r="B83" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
@@ -2221,10 +2539,12 @@
       <c r="P83" s="6"/>
       <c r="Q83" s="6"/>
     </row>
-    <row r="84" spans="2:17" ht="17">
+    <row r="84" spans="1:17" ht="17">
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
-      <c r="D84" s="8"/>
+      <c r="D84" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
       <c r="G84" s="8"/>
@@ -2239,7 +2559,7 @@
       <c r="P84" s="6"/>
       <c r="Q84" s="6"/>
     </row>
-    <row r="85" spans="2:17" ht="17">
+    <row r="85" spans="1:17" ht="17">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="8"/>
@@ -2257,7 +2577,7 @@
       <c r="P85" s="6"/>
       <c r="Q85" s="6"/>
     </row>
-    <row r="86" spans="2:17" ht="17">
+    <row r="86" spans="1:17" ht="17">
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="8"/>
@@ -2275,7 +2595,7 @@
       <c r="P86" s="6"/>
       <c r="Q86" s="6"/>
     </row>
-    <row r="87" spans="2:17" ht="17">
+    <row r="87" spans="1:17" ht="17">
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="8"/>
@@ -2293,7 +2613,7 @@
       <c r="P87" s="6"/>
       <c r="Q87" s="6"/>
     </row>
-    <row r="88" spans="2:17" ht="17">
+    <row r="88" spans="1:17" ht="17">
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="8"/>
@@ -2311,7 +2631,7 @@
       <c r="P88" s="6"/>
       <c r="Q88" s="6"/>
     </row>
-    <row r="89" spans="2:17" ht="17">
+    <row r="89" spans="1:17" ht="17">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="8"/>
@@ -2329,9 +2649,16 @@
       <c r="P89" s="6"/>
       <c r="Q89" s="6"/>
     </row>
-    <row r="90" spans="2:17" ht="17">
-      <c r="B90" s="10"/>
-      <c r="C90" s="12"/>
+    <row r="90" spans="1:17" ht="17">
+      <c r="A90">
+        <v>20</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
@@ -2346,13 +2673,21 @@
       <c r="P90" s="6"/>
       <c r="Q90" s="6"/>
     </row>
-    <row r="91" spans="2:17" ht="17">
+    <row r="91" spans="1:17" ht="17">
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
-      <c r="D91" s="12"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="12"/>
+      <c r="D91" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E91" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F91" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="H91" s="12"/>
       <c r="I91" s="12"/>
       <c r="J91" s="7"/>
@@ -2364,13 +2699,21 @@
       <c r="P91" s="6"/>
       <c r="Q91" s="6"/>
     </row>
-    <row r="92" spans="2:17" ht="17">
+    <row r="92" spans="1:17" ht="17">
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
-      <c r="D92" s="12"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
+      <c r="D92" s="12">
+        <v>7</v>
+      </c>
+      <c r="E92" s="12">
+        <v>5</v>
+      </c>
+      <c r="F92" s="12">
+        <v>3</v>
+      </c>
+      <c r="G92" s="12">
+        <v>1</v>
+      </c>
       <c r="H92" s="12"/>
       <c r="I92" s="12"/>
       <c r="J92" s="7"/>
@@ -2382,7 +2725,7 @@
       <c r="P92" s="6"/>
       <c r="Q92" s="6"/>
     </row>
-    <row r="93" spans="2:17" ht="17">
+    <row r="93" spans="1:17" ht="17">
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
       <c r="D93" s="12"/>
@@ -2400,9 +2743,16 @@
       <c r="P93" s="6"/>
       <c r="Q93" s="6"/>
     </row>
-    <row r="94" spans="2:17" ht="17">
-      <c r="B94" s="10"/>
-      <c r="C94" s="12"/>
+    <row r="94" spans="1:17" ht="17">
+      <c r="A94">
+        <v>21</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="E94" s="12"/>
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
@@ -2417,14 +2767,24 @@
       <c r="P94" s="6"/>
       <c r="Q94" s="6"/>
     </row>
-    <row r="95" spans="2:17" ht="17">
+    <row r="95" spans="1:17" ht="17">
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
-      <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="12"/>
+      <c r="D95" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G95" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H95" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="I95" s="13"/>
       <c r="J95" s="5"/>
       <c r="K95" s="7"/>
@@ -2435,13 +2795,21 @@
       <c r="P95" s="6"/>
       <c r="Q95" s="6"/>
     </row>
-    <row r="96" spans="2:17" ht="17">
+    <row r="96" spans="1:17" ht="17">
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
-      <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="12"/>
+      <c r="D96" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G96" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
       <c r="J96" s="5"/>
@@ -2453,7 +2821,7 @@
       <c r="P96" s="6"/>
       <c r="Q96" s="6"/>
     </row>
-    <row r="97" spans="2:17" ht="17">
+    <row r="97" spans="1:17" ht="17">
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="12"/>
@@ -2471,7 +2839,7 @@
       <c r="P97" s="6"/>
       <c r="Q97" s="6"/>
     </row>
-    <row r="98" spans="2:17" ht="17">
+    <row r="98" spans="1:17" ht="17">
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="12"/>
@@ -2489,9 +2857,16 @@
       <c r="P98" s="6"/>
       <c r="Q98" s="6"/>
     </row>
-    <row r="99" spans="2:17" ht="17">
-      <c r="B99" s="10"/>
-      <c r="C99" s="12"/>
+    <row r="99" spans="1:17" ht="17">
+      <c r="A99">
+        <v>22</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
@@ -2506,10 +2881,12 @@
       <c r="P99" s="6"/>
       <c r="Q99" s="6"/>
     </row>
-    <row r="100" spans="2:17" ht="17">
+    <row r="100" spans="1:17" ht="17">
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
-      <c r="D100" s="12"/>
+      <c r="D100" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="E100" s="12"/>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
@@ -2524,7 +2901,7 @@
       <c r="P100" s="6"/>
       <c r="Q100" s="6"/>
     </row>
-    <row r="101" spans="2:17" ht="17">
+    <row r="101" spans="1:17" ht="17">
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
       <c r="D101" s="12"/>
@@ -2542,7 +2919,7 @@
       <c r="P101" s="6"/>
       <c r="Q101" s="6"/>
     </row>
-    <row r="102" spans="2:17" ht="17">
+    <row r="102" spans="1:17" ht="17">
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
       <c r="D102" s="12"/>
@@ -2560,9 +2937,16 @@
       <c r="P102" s="6"/>
       <c r="Q102" s="6"/>
     </row>
-    <row r="103" spans="2:17" ht="17">
-      <c r="B103" s="10"/>
-      <c r="C103" s="12"/>
+    <row r="103" spans="1:17" ht="17">
+      <c r="A103">
+        <v>23</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E103" s="12"/>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
@@ -2577,10 +2961,12 @@
       <c r="P103" s="6"/>
       <c r="Q103" s="6"/>
     </row>
-    <row r="104" spans="2:17" ht="17">
+    <row r="104" spans="1:17" ht="17">
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
-      <c r="D104" s="12"/>
+      <c r="D104" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="E104" s="12"/>
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
@@ -2595,7 +2981,7 @@
       <c r="P104" s="6"/>
       <c r="Q104" s="6"/>
     </row>
-    <row r="105" spans="2:17">
+    <row r="105" spans="1:17">
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
@@ -2608,7 +2994,7 @@
       <c r="K105" s="11"/>
       <c r="L105" s="11"/>
     </row>
-    <row r="106" spans="2:17">
+    <row r="106" spans="1:17">
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
@@ -2621,7 +3007,7 @@
       <c r="K106" s="11"/>
       <c r="L106" s="11"/>
     </row>
-    <row r="107" spans="2:17">
+    <row r="107" spans="1:17">
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
@@ -2634,7 +3020,7 @@
       <c r="K107" s="11"/>
       <c r="L107" s="11"/>
     </row>
-    <row r="108" spans="2:17">
+    <row r="108" spans="1:17">
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
@@ -2647,7 +3033,7 @@
       <c r="K108" s="11"/>
       <c r="L108" s="11"/>
     </row>
-    <row r="109" spans="2:17">
+    <row r="109" spans="1:17">
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
@@ -2660,7 +3046,7 @@
       <c r="K109" s="11"/>
       <c r="L109" s="11"/>
     </row>
-    <row r="110" spans="2:17">
+    <row r="110" spans="1:17">
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
@@ -2673,7 +3059,7 @@
       <c r="K110" s="11"/>
       <c r="L110" s="11"/>
     </row>
-    <row r="111" spans="2:17">
+    <row r="111" spans="1:17">
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>

</xml_diff>

<commit_message>
End of play Saturday
</commit_message>
<xml_diff>
--- a/Python/src/_Highlands/questions.xlsx
+++ b/Python/src/_Highlands/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Question</t>
   </si>
@@ -190,15 +190,6 @@
   </si>
   <si>
     <t>In the past year</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>client</t>
-  </si>
-  <si>
-    <t>blank</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1115,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1327,7 +1318,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="17">
+    <row r="17" spans="1:18" ht="17">
       <c r="A17" s="17">
         <v>4</v>
       </c>
@@ -1343,7 +1334,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="17">
+    <row r="18" spans="1:18" ht="17">
       <c r="C18" s="14"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
@@ -1352,14 +1343,14 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="17">
+    <row r="19" spans="1:18" ht="17">
       <c r="C19" s="14"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="17">
+    <row r="20" spans="1:18" ht="17">
       <c r="A20" s="17">
         <v>5</v>
       </c>
@@ -1375,7 +1366,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:18">
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13" t="s">
@@ -1384,164 +1375,236 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:18">
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:18" ht="17">
       <c r="A23" s="17">
-        <v>6</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="13"/>
+        <v>11</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13">
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13" t="s">
-        <v>59</v>
+    <row r="24" spans="1:18" ht="17">
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13">
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
+    <row r="25" spans="1:18" ht="17">
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="19">
+        <v>10</v>
+      </c>
+      <c r="G25" s="19">
+        <v>8</v>
+      </c>
+      <c r="H25" s="19">
+        <v>5</v>
+      </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13">
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+    <row r="26" spans="1:18" ht="17">
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="19">
+        <v>9</v>
+      </c>
+      <c r="G26" s="19">
+        <v>7</v>
+      </c>
+      <c r="H26" s="18">
+        <v>3</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13">
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+    <row r="27" spans="1:18" ht="17">
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="19">
+        <v>6</v>
+      </c>
+      <c r="G27" s="18">
+        <v>3</v>
+      </c>
+      <c r="H27" s="18">
+        <v>1</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="17">
-      <c r="A28" s="17">
-        <v>11</v>
-      </c>
-      <c r="B28" s="17" t="s">
+    <row r="28" spans="1:18" ht="17">
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="18">
+        <v>2</v>
+      </c>
+      <c r="G28" s="18">
+        <v>1</v>
+      </c>
+      <c r="H28" s="18">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+    </row>
+    <row r="29" spans="1:18" ht="17">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+    </row>
+    <row r="30" spans="1:18" ht="17">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+    </row>
+    <row r="31" spans="1:18" ht="17">
+      <c r="A31" s="17">
+        <v>32</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="1:13" ht="17">
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" ht="17">
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="19">
+      <c r="C31" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="19">
-        <v>8</v>
-      </c>
-      <c r="H30" s="19">
-        <v>5</v>
-      </c>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13" ht="17">
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="19">
-        <v>9</v>
-      </c>
-      <c r="G31" s="19">
-        <v>7</v>
-      </c>
-      <c r="H31" s="18">
-        <v>3</v>
-      </c>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:13" ht="17">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+    </row>
+    <row r="32" spans="1:18" ht="17">
       <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="19">
-        <v>6</v>
-      </c>
-      <c r="G32" s="18">
-        <v>3</v>
-      </c>
-      <c r="H32" s="18">
-        <v>1</v>
-      </c>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
     </row>
     <row r="33" spans="1:18" ht="17">
       <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="18">
-        <v>2</v>
-      </c>
-      <c r="G33" s="18">
-        <v>1</v>
-      </c>
-      <c r="H33" s="18">
-        <v>0</v>
-      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11">
+        <v>7</v>
+      </c>
+      <c r="F33" s="11">
+        <v>3</v>
+      </c>
+      <c r="G33" s="11">
+        <v>5</v>
+      </c>
+      <c r="H33" s="11"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="K33" s="8"/>
@@ -1554,12 +1617,10 @@
       <c r="R33" s="6"/>
     </row>
     <row r="34" spans="1:18" ht="17">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
@@ -1574,12 +1635,19 @@
       <c r="R34" s="6"/>
     </row>
     <row r="35" spans="1:18" ht="17">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+      <c r="A35" s="17">
+        <v>33</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
@@ -1594,19 +1662,11 @@
       <c r="R35" s="6"/>
     </row>
     <row r="36" spans="1:18" ht="17">
-      <c r="A36" s="17">
-        <v>32</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="11"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
@@ -1625,14 +1685,10 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>15</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
@@ -1648,14 +1704,14 @@
     <row r="38" spans="1:18" ht="17">
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="11">
-        <v>7</v>
-      </c>
-      <c r="F38" s="11">
-        <v>3</v>
-      </c>
-      <c r="G38" s="11">
-        <v>5</v>
+      <c r="E38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
@@ -1672,9 +1728,15 @@
     <row r="39" spans="1:18" ht="17">
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
+      <c r="E39" s="11">
+        <v>0</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
@@ -1688,18 +1750,9 @@
       <c r="R39" s="6"/>
     </row>
     <row r="40" spans="1:18" ht="17">
-      <c r="A40" s="17">
-        <v>33</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
@@ -1715,11 +1768,19 @@
       <c r="R40" s="6"/>
     </row>
     <row r="41" spans="1:18" ht="17">
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11" t="s">
-        <v>16</v>
-      </c>
+      <c r="A41" s="17">
+        <v>34</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
@@ -1734,15 +1795,16 @@
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
     </row>
-    <row r="42" spans="1:18" ht="17">
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+    <row r="42" spans="1:18">
+      <c r="E42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" t="s">
+        <v>33</v>
+      </c>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="8"/>
@@ -1754,19 +1816,16 @@
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
     </row>
-    <row r="43" spans="1:18" ht="17">
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="11"/>
+    <row r="43" spans="1:18">
+      <c r="E43" s="16">
+        <v>3</v>
+      </c>
+      <c r="F43" s="16">
+        <v>7</v>
+      </c>
+      <c r="G43" s="16">
+        <v>9</v>
+      </c>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="K43" s="8"/>
@@ -1779,20 +1838,14 @@
       <c r="R43" s="6"/>
     </row>
     <row r="44" spans="1:18" ht="17">
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="11">
-        <v>0</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="M44" s="7"/>
@@ -1803,14 +1856,14 @@
       <c r="R44" s="6"/>
     </row>
     <row r="45" spans="1:18" ht="17">
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
       <c r="M45" s="7"/>
@@ -1820,25 +1873,9 @@
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="1:18" ht="17">
-      <c r="A46" s="17">
-        <v>34</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
+    <row r="46" spans="1:18">
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="7"/>
@@ -1849,17 +1886,8 @@
       <c r="R46" s="6"/>
     </row>
     <row r="47" spans="1:18">
-      <c r="E47" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" t="s">
-        <v>33</v>
-      </c>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
       <c r="M47" s="7"/>
@@ -1869,18 +1897,19 @@
       <c r="Q47" s="6"/>
       <c r="R47" s="6"/>
     </row>
-    <row r="48" spans="1:18">
-      <c r="E48" s="16">
-        <v>3</v>
-      </c>
-      <c r="F48" s="16">
-        <v>7</v>
-      </c>
-      <c r="G48" s="16">
-        <v>9</v>
-      </c>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
+    <row r="48" spans="1:18" ht="17">
+      <c r="C48" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="7"/>
@@ -1893,7 +1922,9 @@
     <row r="49" spans="3:18" ht="17">
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
-      <c r="E49" s="8"/>
+      <c r="E49" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
@@ -1926,90 +1957,6 @@
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
     </row>
-    <row r="51" spans="3:18">
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
-    </row>
-    <row r="52" spans="3:18">
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
-    </row>
-    <row r="53" spans="3:18" ht="17">
-      <c r="C53" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-      <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
-    </row>
-    <row r="54" spans="3:18" ht="17">
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
-    </row>
-    <row r="55" spans="3:18" ht="17">
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
changed chart to display each db record
</commit_message>
<xml_diff>
--- a/Python/src/_Highlands/questions.xlsx
+++ b/Python/src/_Highlands/questions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Please describe the business impact in terms of how it will impact key business measurements of importance to their board.</t>
   </si>
   <si>
-    <t>Please enter "X,Y"  (X = Market Growth), Y = Client Revenue Growth): Major Decline = 0, Flat = 5, Very Strong = 10</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -532,6 +529,9 @@
   </si>
   <si>
     <t>textarea</t>
+  </si>
+  <si>
+    <t>Please enter "X,Y"  (X = Market Growth), Y = Client Revenue Growth):</t>
   </si>
 </sst>
 </file>
@@ -1559,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="D178" sqref="D178"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1572,16 +1572,16 @@
   <sheetData>
     <row r="1" spans="1:13" ht="60" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -1633,10 +1633,10 @@
     </row>
     <row r="4" spans="1:13" ht="51" customHeight="1">
       <c r="C4" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="15"/>
       <c r="L4" s="1"/>
@@ -1646,7 +1646,7 @@
       <c r="C5" s="27"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1670,13 +1670,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>72</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1685,7 +1685,7 @@
       <c r="C9" s="27"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1702,13 +1702,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1717,7 +1717,7 @@
       <c r="C12" s="27"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1734,13 +1734,13 @@
         <v>3</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1749,7 +1749,7 @@
       <c r="C15" s="27"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1766,13 +1766,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1781,7 +1781,7 @@
       <c r="C18" s="27"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1798,13 +1798,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1813,7 +1813,7 @@
       <c r="C21" s="26"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1862,10 +1862,10 @@
     </row>
     <row r="28" spans="1:13" ht="59" customHeight="1">
       <c r="C28" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" s="15"/>
       <c r="L28" s="1"/>
@@ -1875,7 +1875,7 @@
       <c r="C29" s="26"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -1892,10 +1892,10 @@
         <v>6</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E31" s="15"/>
       <c r="L31" s="1"/>
@@ -1905,7 +1905,7 @@
       <c r="C32" s="27"/>
       <c r="D32" s="15"/>
       <c r="E32" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -1922,7 +1922,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>19</v>
@@ -1935,7 +1935,7 @@
       <c r="C35" s="26"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -1977,10 +1977,10 @@
     </row>
     <row r="43" spans="1:18" ht="17">
       <c r="C43" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E43" s="15"/>
       <c r="L43" s="1"/>
@@ -1990,7 +1990,7 @@
       <c r="C44" s="30"/>
       <c r="D44" s="16"/>
       <c r="E44" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
@@ -2019,10 +2019,10 @@
         <v>8</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>18</v>
@@ -2112,10 +2112,10 @@
         <v>9</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>18</v>
@@ -2217,10 +2217,10 @@
         <v>10</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>18</v>
@@ -2314,10 +2314,10 @@
         <v>11</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>18</v>
@@ -2403,10 +2403,10 @@
         <v>12</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>18</v>
@@ -2496,10 +2496,10 @@
         <v>13</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>18</v>
@@ -2585,10 +2585,10 @@
         <v>14</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>18</v>
@@ -2678,10 +2678,10 @@
         <v>15</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>18</v>
@@ -2767,10 +2767,10 @@
         <v>16</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>18</v>
@@ -2860,10 +2860,10 @@
         <v>17</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C82" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>18</v>
@@ -2953,10 +2953,10 @@
         <v>18</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C86" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>18</v>
@@ -3054,10 +3054,10 @@
         <v>19</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C90" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>18</v>
@@ -3159,10 +3159,10 @@
         <v>20</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C94" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>18</v>
@@ -3194,10 +3194,10 @@
         <v>46</v>
       </c>
       <c r="H95" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I95" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="I95" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="J95" s="8"/>
       <c r="K95" s="8"/>
@@ -3260,10 +3260,10 @@
         <v>21</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C98" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>18</v>
@@ -3287,16 +3287,16 @@
       <c r="C99" s="32"/>
       <c r="D99" s="9"/>
       <c r="E99" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F99" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F99" s="8" t="s">
+      <c r="G99" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G99" s="8" t="s">
+      <c r="H99" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="H99" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="I99" s="8"/>
       <c r="J99" s="8"/>
@@ -3427,10 +3427,10 @@
     </row>
     <row r="106" spans="1:18" ht="17">
       <c r="C106" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="8"/>
@@ -3451,7 +3451,7 @@
       <c r="C107" s="32"/>
       <c r="D107" s="9"/>
       <c r="E107" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F107" s="8"/>
       <c r="G107" s="8"/>
@@ -3490,10 +3490,10 @@
         <v>22</v>
       </c>
       <c r="B109" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D109" s="12" t="s">
         <v>18</v>
@@ -3587,10 +3587,10 @@
         <v>23</v>
       </c>
       <c r="B113" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D113" s="12" t="s">
         <v>18</v>
@@ -3613,13 +3613,13 @@
       <c r="C114" s="31"/>
       <c r="D114" s="10"/>
       <c r="E114" t="s">
+        <v>104</v>
+      </c>
+      <c r="F114" t="s">
         <v>105</v>
       </c>
-      <c r="F114" t="s">
+      <c r="G114" t="s">
         <v>106</v>
-      </c>
-      <c r="G114" t="s">
-        <v>107</v>
       </c>
       <c r="J114" s="13"/>
       <c r="K114" s="8"/>
@@ -3676,10 +3676,10 @@
         <v>24</v>
       </c>
       <c r="B117" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C117" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D117" s="12" t="s">
         <v>18</v>
@@ -3703,19 +3703,19 @@
       <c r="C118" s="31"/>
       <c r="D118" s="10"/>
       <c r="E118" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F118" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F118" s="12" t="s">
+      <c r="G118" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G118" s="12" t="s">
+      <c r="H118" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H118" s="12" t="s">
+      <c r="I118" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="I118" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="J118" s="12"/>
       <c r="K118" s="8"/>
@@ -3778,10 +3778,10 @@
         <v>25</v>
       </c>
       <c r="B121" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C121" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D121" s="12" t="s">
         <v>18</v>
@@ -3805,19 +3805,19 @@
       <c r="C122" s="31"/>
       <c r="D122" s="10"/>
       <c r="E122" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F122" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="F122" s="12" t="s">
+      <c r="G122" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G122" s="12" t="s">
+      <c r="H122" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="H122" s="12" t="s">
+      <c r="I122" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="I122" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="J122" s="12" t="s">
         <v>30</v>
@@ -3884,10 +3884,10 @@
         <v>26</v>
       </c>
       <c r="B125" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C125" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D125" s="12" t="s">
         <v>21</v>
@@ -3911,7 +3911,7 @@
       <c r="C126" s="31"/>
       <c r="D126" s="12"/>
       <c r="E126" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F126" s="22" t="s">
         <v>48</v>
@@ -3923,7 +3923,7 @@
         <v>50</v>
       </c>
       <c r="I126" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J126" s="12"/>
       <c r="K126" s="8"/>
@@ -4088,10 +4088,10 @@
         <v>27</v>
       </c>
       <c r="B133" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D133" s="12" t="s">
         <v>18</v>
@@ -4177,10 +4177,10 @@
         <v>28</v>
       </c>
       <c r="B137" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C137" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D137" s="12" t="s">
         <v>18</v>
@@ -4267,10 +4267,10 @@
         <v>29</v>
       </c>
       <c r="B141" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C141" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D141" s="12" t="s">
         <v>18</v>
@@ -4357,10 +4357,10 @@
         <v>30</v>
       </c>
       <c r="B145" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D145" s="12" t="s">
         <v>18</v>
@@ -4447,10 +4447,10 @@
         <v>31</v>
       </c>
       <c r="B149" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C149" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D149" s="12" t="s">
         <v>18</v>
@@ -4541,10 +4541,10 @@
         <v>32</v>
       </c>
       <c r="B153" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C153" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D153" s="12" t="s">
         <v>18</v>
@@ -4635,10 +4635,10 @@
         <v>33</v>
       </c>
       <c r="B157" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C157" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D157" s="12" t="s">
         <v>20</v>
@@ -4661,7 +4661,7 @@
       <c r="C158" s="31"/>
       <c r="D158" s="10"/>
       <c r="E158" s="12" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F158" s="12"/>
       <c r="G158" s="12"/>
@@ -4681,7 +4681,7 @@
       <c r="C159" s="31"/>
       <c r="D159" s="10"/>
       <c r="E159" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F159" s="12"/>
       <c r="G159" s="12"/>
@@ -4701,13 +4701,13 @@
       <c r="C160" s="31"/>
       <c r="D160" s="10"/>
       <c r="E160" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F160" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="F160" s="12" t="s">
+      <c r="G160" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="G160" s="12" t="s">
-        <v>165</v>
       </c>
       <c r="H160" s="12"/>
       <c r="I160" s="12"/>
@@ -4728,10 +4728,10 @@
         <v>0</v>
       </c>
       <c r="F161" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G161" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H161" s="12"/>
       <c r="I161" s="12"/>
@@ -4768,10 +4768,10 @@
         <v>34</v>
       </c>
       <c r="B163" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C163" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D163" s="12" t="s">
         <v>18</v>
@@ -4793,13 +4793,13 @@
     </row>
     <row r="164" spans="1:18">
       <c r="E164" t="s">
+        <v>107</v>
+      </c>
+      <c r="F164" t="s">
         <v>108</v>
       </c>
-      <c r="F164" t="s">
+      <c r="G164" t="s">
         <v>109</v>
-      </c>
-      <c r="G164" t="s">
-        <v>110</v>
       </c>
       <c r="I164" s="12"/>
       <c r="J164" s="12"/>
@@ -4955,10 +4955,10 @@
     </row>
     <row r="174" spans="1:18" ht="17">
       <c r="C174" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E174" s="8"/>
       <c r="F174" s="8"/>
@@ -4979,7 +4979,7 @@
       <c r="C175" s="32"/>
       <c r="D175" s="9"/>
       <c r="E175" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F175" s="8"/>
       <c r="G175" s="8"/>
@@ -5018,10 +5018,10 @@
         <v>35</v>
       </c>
       <c r="C177" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D177" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E177" s="8"/>
       <c r="F177" s="8"/>
@@ -5078,13 +5078,13 @@
         <v>36</v>
       </c>
       <c r="B180" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C180" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D180" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K180" s="7"/>
       <c r="L180" s="7"/>
@@ -5097,22 +5097,22 @@
     </row>
     <row r="181" spans="1:18">
       <c r="E181" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F181" t="s">
+        <v>114</v>
+      </c>
+      <c r="G181" t="s">
         <v>115</v>
       </c>
-      <c r="G181" t="s">
+      <c r="H181" t="s">
         <v>116</v>
       </c>
-      <c r="H181" t="s">
+      <c r="I181" t="s">
         <v>117</v>
       </c>
-      <c r="I181" t="s">
+      <c r="J181" t="s">
         <v>118</v>
-      </c>
-      <c r="J181" t="s">
-        <v>119</v>
       </c>
       <c r="K181" s="7"/>
       <c r="L181" s="7"/>
@@ -5166,10 +5166,10 @@
         <v>37</v>
       </c>
       <c r="B184" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C184" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D184" s="12" t="s">
         <v>18</v>
@@ -5240,10 +5240,10 @@
         <v>38</v>
       </c>
       <c r="B188" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C188" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D188" s="12" t="s">
         <v>18</v>
@@ -5318,10 +5318,10 @@
         <v>39</v>
       </c>
       <c r="B192" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C192" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D192" s="12" t="s">
         <v>18</v>
@@ -5396,10 +5396,10 @@
         <v>40</v>
       </c>
       <c r="B196" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C196" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D196" s="12" t="s">
         <v>18</v>
@@ -5470,10 +5470,10 @@
         <v>41</v>
       </c>
       <c r="B200" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C200" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D200" s="11" t="s">
         <v>21</v>
@@ -5491,7 +5491,7 @@
     <row r="201" spans="1:18" ht="17">
       <c r="C201" s="27"/>
       <c r="E201" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F201" s="22" t="s">
         <v>27</v>
@@ -5506,7 +5506,7 @@
     <row r="202" spans="1:18" ht="17">
       <c r="C202" s="27"/>
       <c r="E202" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F202" s="20">
         <v>10</v>
@@ -5521,7 +5521,7 @@
     <row r="203" spans="1:18" ht="17">
       <c r="C203" s="27"/>
       <c r="E203" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F203" s="20">
         <v>9</v>
@@ -5536,7 +5536,7 @@
     <row r="204" spans="1:18" ht="17">
       <c r="C204" s="27"/>
       <c r="E204" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F204" s="20">
         <v>6</v>
@@ -5560,10 +5560,10 @@
         <v>42</v>
       </c>
       <c r="B206" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C206" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D206" s="12" t="s">
         <v>18</v>
@@ -5606,31 +5606,31 @@
         <v>43</v>
       </c>
       <c r="B210" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C210" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D210" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="211" spans="1:9" ht="17">
       <c r="C211" s="27"/>
       <c r="E211" t="s">
+        <v>123</v>
+      </c>
+      <c r="F211" t="s">
         <v>124</v>
       </c>
-      <c r="F211" t="s">
+      <c r="G211" t="s">
         <v>125</v>
       </c>
-      <c r="G211" t="s">
+      <c r="H211" t="s">
         <v>126</v>
       </c>
-      <c r="H211" t="s">
+      <c r="I211" t="s">
         <v>127</v>
-      </c>
-      <c r="I211" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="212" spans="1:9" ht="17">
@@ -5659,16 +5659,16 @@
         <v>44</v>
       </c>
       <c r="B214" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C214" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D214" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E214" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F214" s="22" t="s">
         <v>27</v>
@@ -5683,7 +5683,7 @@
     <row r="215" spans="1:9" ht="17">
       <c r="C215" s="27"/>
       <c r="E215" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F215" s="20">
         <v>7</v>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="216" spans="1:9">
       <c r="E216" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F216" s="20">
         <v>8</v>
@@ -5711,7 +5711,7 @@
     </row>
     <row r="217" spans="1:9">
       <c r="E217" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F217" s="20">
         <v>6</v>
@@ -5725,7 +5725,7 @@
     </row>
     <row r="218" spans="1:9">
       <c r="E218" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F218" s="20">
         <v>4</v>
@@ -5739,7 +5739,7 @@
     </row>
     <row r="219" spans="1:9">
       <c r="E219" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F219" s="20">
         <v>9</v>
@@ -5753,7 +5753,7 @@
     </row>
     <row r="220" spans="1:9">
       <c r="E220" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F220" s="20">
         <v>8</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="221" spans="1:9">
       <c r="E221" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F221" s="20">
         <v>6</v>

</xml_diff>